<commit_message>
Changes in Slot Generation Test
</commit_message>
<xml_diff>
--- a/inputFiles/Doctor_Login.xlsx
+++ b/inputFiles/Doctor_Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\EzscheulerProject\EzScheduler\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4AFBE8-F80A-4AC4-B93E-656FE3BA8A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C9B09D-92D6-4C5B-84E9-7C5A7D1CA695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="109">
   <si>
     <t>UserName</t>
   </si>
@@ -340,9 +340,6 @@
     <t>21122021</t>
   </si>
   <si>
-    <t>09122021</t>
-  </si>
-  <si>
     <t>07122021</t>
   </si>
   <si>
@@ -350,6 +347,12 @@
   </si>
   <si>
     <t>11122021</t>
+  </si>
+  <si>
+    <t>9122021</t>
+  </si>
+  <si>
+    <t>7122021</t>
   </si>
 </sst>
 </file>
@@ -794,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,10 +1037,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
         <v>66</v>
@@ -1069,10 +1072,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s">
         <v>85</v>
@@ -1104,10 +1107,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
         <v>66</v>
@@ -1137,10 +1140,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
         <v>66</v>

</xml_diff>